<commit_message>
Getting to the ACF
</commit_message>
<xml_diff>
--- a/Root_hours.xlsx
+++ b/Root_hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDSFSSkatter\Documents\Personal\spore_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0F0581-5711-472A-BDDB-EAB5045A8EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2F856-4B09-4A25-BD32-400B934B12E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Import and prep data</t>
+  </si>
+  <si>
+    <t>More prepping, getting towards temp ACF</t>
   </si>
 </sst>
 </file>
@@ -358,16 +361,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="46.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -401,6 +404,17 @@
       </c>
       <c r="C3">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making an image repre of data
</commit_message>
<xml_diff>
--- a/Root_hours.xlsx
+++ b/Root_hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDSFSSkatter\Documents\Personal\spore_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2F856-4B09-4A25-BD32-400B934B12E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3BB13A-1711-4147-85AD-C18232ADAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>More prepping, getting towards temp ACF</t>
+  </si>
+  <si>
+    <t>Starting on the spatial ACF</t>
+  </si>
+  <si>
+    <t>Mapping the overall data trends</t>
   </si>
 </sst>
 </file>
@@ -361,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -414,7 +420,29 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More elaborate schemes for ACF
</commit_message>
<xml_diff>
--- a/Root_hours.xlsx
+++ b/Root_hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDSFSSkatter\Documents\Personal\spore_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3BB13A-1711-4147-85AD-C18232ADAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF178FE0-9ECE-4F6E-87C1-AA7716417EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Mapping the overall data trends</t>
+  </si>
+  <si>
+    <t>Trying various approaches for spatial ACF</t>
   </si>
 </sst>
 </file>
@@ -367,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,6 +448,17 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>44903</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizing the ACF computes, saving graphs
</commit_message>
<xml_diff>
--- a/Root_hours.xlsx
+++ b/Root_hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDSFSSkatter\Documents\Personal\spore_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF178FE0-9ECE-4F6E-87C1-AA7716417EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0489D4-37BF-42DB-AC44-8398AB74F30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Trying various approaches for spatial ACF</t>
+  </si>
+  <si>
+    <t>Finalizing all the ACFs</t>
+  </si>
+  <si>
+    <t>Write report</t>
   </si>
 </sst>
 </file>
@@ -370,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,6 +465,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>44904</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Invoiced for initial work
</commit_message>
<xml_diff>
--- a/Root_hours.xlsx
+++ b/Root_hours.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDSFSSkatter\Documents\Personal\spore_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a318e94bead91bf/Documents/projects/root_applied_sciences/spore_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0291A202-80D2-4D6F-A5F8-20E593C0AA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{0291A202-80D2-4D6F-A5F8-20E593C0AA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F19DC9F-E74A-4848-AEFF-0DC01DA66984}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -61,14 +73,74 @@
   </si>
   <si>
     <t>Finish report</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From </t>
+  </si>
+  <si>
+    <t>Sondre Skatter</t>
+  </si>
+  <si>
+    <t>6225 Brookside Ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To </t>
+  </si>
+  <si>
+    <t>Total hours</t>
+  </si>
+  <si>
+    <t>Invoice total</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Hourly Rate</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Root Applied Sciences</t>
+  </si>
+  <si>
+    <t>Spore Data Analysis</t>
+  </si>
+  <si>
+    <t>Oakland, CA 94618</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -92,15 +164,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,17 +530,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,7 +551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44901</v>
       </c>
@@ -413,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44901</v>
       </c>
@@ -424,7 +573,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44902</v>
       </c>
@@ -435,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44902</v>
       </c>
@@ -446,7 +595,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44902</v>
       </c>
@@ -457,7 +606,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44903</v>
       </c>
@@ -468,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44904</v>
       </c>
@@ -479,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44904</v>
       </c>
@@ -490,7 +639,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44904</v>
       </c>
@@ -499,6 +648,270 @@
       </c>
       <c r="C10">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6E7EC6-8007-4DE3-9497-640CE41E353A}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="43.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44570</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <f>C26</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B9*D14</f>
+        <v>2550</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44901</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <f>C15*D$14</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44901</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>1.5</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" ref="D16:D23" si="0">C16*D$14</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44903</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44904</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44904</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>1.5</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44904</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="12">
+        <f>SUM(C15:C25)</f>
+        <v>17</v>
+      </c>
+      <c r="D26" s="13">
+        <f>C26*D14</f>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating more graphs for Julian
</commit_message>
<xml_diff>
--- a/Root_hours.xlsx
+++ b/Root_hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a318e94bead91bf/Documents/projects/root_applied_sciences/spore_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{0291A202-80D2-4D6F-A5F8-20E593C0AA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F19DC9F-E74A-4848-AEFF-0DC01DA66984}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{0291A202-80D2-4D6F-A5F8-20E593C0AA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56F21C15-5436-41C5-BDDE-19ED30D5053C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="1740" windowWidth="20292" windowHeight="9336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Oakland, CA 94618</t>
+  </si>
+  <si>
+    <t>Adding plots for equal bin sizes</t>
   </si>
 </sst>
 </file>
@@ -660,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6E7EC6-8007-4DE3-9497-640CE41E353A}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +716,7 @@
       </c>
       <c r="B9">
         <f>C26</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -722,7 +725,7 @@
       </c>
       <c r="B10" s="3">
         <f>B9*D14</f>
-        <v>2550</v>
+        <v>2700</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -778,7 +781,7 @@
         <v>1.5</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" ref="D16:D23" si="0">C16*D$14</f>
+        <f t="shared" ref="D16:D24" si="0">C16*D$14</f>
         <v>225</v>
       </c>
     </row>
@@ -888,8 +891,19 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="D24" s="9"/>
+      <c r="A24" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
@@ -902,11 +916,11 @@
       </c>
       <c r="C26" s="12">
         <f>SUM(C15:C25)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D26" s="13">
         <f>C26*D14</f>
-        <v>2550</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>